<commit_message>
fixed test data sets in epp-11-data
</commit_message>
<xml_diff>
--- a/data/epp-11-data.xlsx
+++ b/data/epp-11-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/icann/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948F5EA7-6613-8940-B893-5B56F53697C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0367D881-11D0-1244-81F2-A5383AF8DF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="49">
   <si>
     <t>errorCode</t>
   </si>
@@ -171,12 +171,6 @@
     <t>NOT::HEX::</t>
   </si>
   <si>
-    <t>192.0.2.2</t>
-  </si>
-  <si>
-    <t>2001:DB8::53:2</t>
-  </si>
-  <si>
     <t>Data Provider for epp-11</t>
   </si>
   <si>
@@ -231,6 +225,12 @@
   </si>
   <si>
     <t>EPP_HOST_CREATE_SERVER_DOES_NOT_REQUIRE_GLUE</t>
+  </si>
+  <si>
+    <t>{"ns2.epp-11.rst." &amp; $TLD}</t>
+  </si>
+  <si>
+    <t>{"ns3.epp-11.rst." &amp; $TLD}</t>
   </si>
 </sst>
 </file>
@@ -344,16 +344,11 @@
   <dxfs count="8">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -394,11 +389,16 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -491,8 +491,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:G31" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B7:G31" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:G29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B7:G29" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -502,11 +502,11 @@
   </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DD252447-D4DE-114E-AF37-9116F81A100C}" name="createParentFirst" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="ip" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DF12F6BB-79CC-F24D-93DC-3FD6FC6C8768}" name="addr" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{DD252447-D4DE-114E-AF37-9116F81A100C}" name="createParentFirst" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="ip" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{DF12F6BB-79CC-F24D-93DC-3FD6FC6C8768}" name="addr" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -829,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:G31"/>
+  <dimension ref="B2:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,7 +849,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -859,7 +859,7 @@
     </row>
     <row r="3" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -895,10 +895,10 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
@@ -915,10 +915,10 @@
     </row>
     <row r="8" spans="2:7" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -938,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>3</v>
@@ -955,10 +955,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -975,66 +975,66 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -1050,8 +1050,11 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -1063,12 +1066,12 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -1080,12 +1083,12 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>23</v>
@@ -1094,12 +1097,12 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1108,12 +1111,12 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
@@ -1122,12 +1125,12 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>18</v>
@@ -1136,12 +1139,12 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>19</v>
@@ -1150,12 +1153,12 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>20</v>
@@ -1170,9 +1173,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>22</v>
@@ -1187,9 +1190,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
@@ -1198,12 +1204,12 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>25</v>
@@ -1212,12 +1218,12 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>26</v>
@@ -1226,12 +1232,12 @@
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>27</v>
@@ -1240,12 +1246,12 @@
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>28</v>
@@ -1254,41 +1260,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revise data providers that compute domain and host names for consistency and to reduce collisions.
</commit_message>
<xml_diff>
--- a/data/epp-11-data.xlsx
+++ b/data/epp-11-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/icann/rst-test-specs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0367D881-11D0-1244-81F2-A5383AF8DF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8BF0EB-F3EF-0F41-996C-B91DF3DC689B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="48">
   <si>
     <t>errorCode</t>
   </si>
@@ -180,12 +180,6 @@
     <t>Hostname</t>
   </si>
   <si>
-    <t>ns1.epp-11.rst.icann</t>
-  </si>
-  <si>
-    <t>{RANDCHARS(64) &amp; ".epp-11.rst." &amp; $TLD}</t>
-  </si>
-  <si>
     <t>EPP_HOST_CREATE_SERVER_ACCEPTS_INVALID_HOSTNAME</t>
   </si>
   <si>
@@ -193,44 +187,48 @@
   </si>
   <si>
     <t>EPP_HOST_CREATE_SERVER_ACCEPTS_INVALID_IPv6_ADDRESS</t>
+  </si>
+  <si>
+    <t>createParentFirst</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Whether the superordinate domain name should be created before the subordinate host name is created (if it does not already exist)</t>
+  </si>
+  <si>
+    <t>EPP_HOST_CREATE_SERVER_DOES_NOT_REQUIRE_GLUE</t>
+  </si>
+  <si>
+    <t>{PREVIOUS}</t>
+  </si>
+  <si>
+    <t>{"ns1.epp-11.rst." &amp; RANDCHARS(18) &amp; ".icann"}</t>
+  </si>
+  <si>
+    <t>{"ns1.epp-11.rst." &amp; RANDCHARS(18) &amp; "." &amp; $TLD}</t>
+  </si>
+  <si>
+    <t>{"!.epp-11.rst." &amp; RANDCHARS(18) &amp; ".icann"}</t>
+  </si>
+  <si>
+    <t>{"ns2.epp-11.rst." &amp; RANDCHARS(18) &amp; "." &amp; $TLD}</t>
+  </si>
+  <si>
+    <t>{"ns3.epp-11.rst." &amp; RANDCHARS(18) &amp; "." &amp; $TLD}</t>
   </si>
   <si>
     <t xml:space="preserve">* Values in {parentheses} are not literal values, they indicate that an appropriate value should be computed.
     * A value of `{EMPTY}` indicates an empty string.
+    * A value of `{PREVIOUS}` indicates that the value computed from the same column in the preceding row should be used.
 </t>
-  </si>
-  <si>
-    <t>{"ns1.epp-11.rst." &amp; $TLD}</t>
-  </si>
-  <si>
-    <t>!.invalid</t>
-  </si>
-  <si>
-    <t>createParentFirst</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Whether the superordinate domain name should be created before the subordinate host name is created (if it does not already exist)</t>
-  </si>
-  <si>
-    <t>{"!.epp-11.rst." &amp; $TLD}</t>
-  </si>
-  <si>
-    <t>EPP_HOST_CREATE_SERVER_DOES_NOT_REQUIRE_GLUE</t>
-  </si>
-  <si>
-    <t>{"ns2.epp-11.rst." &amp; $TLD}</t>
-  </si>
-  <si>
-    <t>{"ns3.epp-11.rst." &amp; $TLD}</t>
   </si>
 </sst>
 </file>
@@ -491,8 +489,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:G29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B7:G29" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:G28" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B7:G28" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -829,16 +827,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:G29"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -857,9 +855,9 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -898,7 +896,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
@@ -918,7 +916,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -938,7 +936,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>3</v>
@@ -955,10 +953,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -975,292 +973,320 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1272,6 +1298,7 @@
     <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>